<commit_message>
update after Manas check
</commit_message>
<xml_diff>
--- a/documentation/input_parameters.xlsx
+++ b/documentation/input_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\GitHub\ember-sim-germany\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8CFE3E-23AC-46F6-B19B-614D0C5A30DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F104B15C-EF74-4606-A097-DF9EA4B094D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EAD22BB8-0710-4D57-B40C-A01F8CC59EE7}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{EAD22BB8-0710-4D57-B40C-A01F8CC59EE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Input Parameters</t>
   </si>
@@ -164,29 +164,50 @@
     <t>North-35.57214862635885, East148.9041407459145, South-35.76257546576715, West148.76542588483267</t>
   </si>
   <si>
-    <t>FRB ???</t>
-  </si>
-  <si>
     <t>Bounds (North, East, South, West)</t>
   </si>
   <si>
     <t>Fire Weather Indices Wiki | Keetch-Byram drought index (wsl.ch)</t>
   </si>
   <si>
-    <t>0-800</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>flat</t>
+  </si>
+  <si>
+    <t>For the KBDI use 150 (see details below)</t>
+  </si>
+  <si>
+    <t>KBDI = 0 - 50: Soil moisture and large class fuel moistures are high and do not contribute much to fire intensity. Typical of spring dormant season following winter precipitation.</t>
+  </si>
+  <si>
+    <t>KBDI = 50 - 100: Typical of late spring, early growing season. Lower litter and duff layers are drying and beginning to contribute to fire intensity.</t>
+  </si>
+  <si>
+    <t>KBDI = 100 - 150: Typical of late summer, early fall. Lower litter and duff layers actively contribute to fire intensity and will burn actively.</t>
+  </si>
+  <si>
+    <t>KBDI = 150 - 200: Often associated with more severe drought with increased wildfire occurrence. Intense, deep burning fires with significant downwind spotting can be expected. Live fuels can also be expected to burn actively at these levels.</t>
+  </si>
+  <si>
+    <t>FRB means if there was fuel reduction burn (FRB) applied to the landscape or not. Because if yes, it reduced the spread of fire. For now use "0" meaning no FRB was applied anywhere.</t>
+  </si>
+  <si>
+    <t>For the parameter w use "1".</t>
+  </si>
+  <si>
+    <t>FRB=Fuel reduction burn</t>
+  </si>
+  <si>
+    <t>0-200</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +235,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -363,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -380,24 +407,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -408,6 +417,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -723,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A92F8D-EEE7-400F-8B40-BEB6E4460687}">
-  <dimension ref="B4:H20"/>
+  <dimension ref="B4:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +781,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -761,34 +789,35 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1">
-        <v>100</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>44</v>
+        <v>150</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -800,11 +829,11 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -818,7 +847,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
@@ -830,7 +859,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -844,7 +873,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
@@ -856,7 +885,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -870,7 +899,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
@@ -894,12 +923,12 @@
       <c r="E15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -913,7 +942,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
@@ -925,11 +954,11 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="7" t="s">
@@ -949,7 +978,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
@@ -958,6 +987,41 @@
       </c>
       <c r="E20" s="4">
         <v>811.13940000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="20" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I do not know, what happend here
</commit_message>
<xml_diff>
--- a/documentation/input_parameters.xlsx
+++ b/documentation/input_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\GitHub\ember-sim-germany\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F104B15C-EF74-4606-A097-DF9EA4B094D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996CF219-2D7A-4E5E-B0D1-2FC88C5478F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{EAD22BB8-0710-4D57-B40C-A01F8CC59EE7}"/>
   </bookViews>
@@ -754,7 +754,7 @@
   <dimension ref="B4:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
upgrade table for parameters
I do not know why I can not commit this with vsc ide.
</commit_message>
<xml_diff>
--- a/documentation/input_parameters.xlsx
+++ b/documentation/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\GitHub\ember-sim-germany\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996CF219-2D7A-4E5E-B0D1-2FC88C5478F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AFD4A7-124E-4193-95F7-29341A8EF15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{EAD22BB8-0710-4D57-B40C-A01F8CC59EE7}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{EAD22BB8-0710-4D57-B40C-A01F8CC59EE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Input Parameters</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Raster extends (x,y)</t>
   </si>
   <si>
-    <t>McArthur Eucalypt</t>
-  </si>
-  <si>
     <t>lat,lng,x,y</t>
   </si>
   <si>
@@ -201,13 +198,28 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>FRB</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>grazing</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>McArthur Eucalypt or Chesey Grassland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +253,12 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -392,21 +410,10 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -417,25 +424,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -751,290 +779,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A92F8D-EEE7-400F-8B40-BEB6E4460687}">
-  <dimension ref="B4:H33"/>
+  <dimension ref="B4:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="76" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="4" width="20.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" customWidth="1"/>
     <col min="7" max="7" width="15.21875" customWidth="1"/>
     <col min="10" max="10" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="E9" s="11">
         <v>150</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="1" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15"/>
+      <c r="C15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="13">
+        <v>50</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="11">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="20"/>
+      <c r="C22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="15"/>
+      <c r="C23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="13">
+        <v>811.13940000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="19"/>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="4">
-        <v>811.13940000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="20" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="20" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="20" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="20" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" display="https://wikifire.wsl.ch/tiki-index908f.html?page=Keetch-Byram+drought+index" xr:uid="{72CB3F46-4EC1-4F3B-B5D4-FBA217D65A1A}"/>
+    <hyperlink ref="F9" r:id="rId1" display="https://wikifire.wsl.ch/tiki-index908f.html?page=Keetch-Byram+drought+index" xr:uid="{72CB3F46-4EC1-4F3B-B5D4-FBA217D65A1A}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>

</xml_diff>